<commit_message>
diary update and minor code ammendments for 50newproteins
</commit_message>
<xml_diff>
--- a/Project/Datasets/GridScores/Combined.xlsx
+++ b/Project/Datasets/GridScores/Combined.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="440" windowWidth="24680" windowHeight="15560" tabRatio="500" activeTab="12"/>
+    <workbookView xWindow="920" yWindow="440" windowWidth="24680" windowHeight="15560" tabRatio="500" firstSheet="1" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="9" sheetId="3" r:id="rId1"/>
@@ -311,7 +311,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="26">
   <si>
     <t>mean_fit_time</t>
   </si>
@@ -533,7 +533,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>WindowComparison!$B$14</c:f>
+              <c:f>WindowComparison!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -566,35 +566,44 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>WindowComparison!$A$15:$A$23</c:f>
+              <c:f>WindowComparison!$A$18:$A$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>15.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>17.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>21.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>23.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>25.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>27.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>29.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>31.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -602,35 +611,44 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>WindowComparison!$B$15:$B$23</c:f>
+              <c:f>WindowComparison!$B$18:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.683766329076765</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.686995449875238</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.693894026126522</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.69976515485102</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>0.70343461030383</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>0.70402172317628</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.704241890503449</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>0.702627330104212</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>0.702700719213268</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>0.702553940995156</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>0.701599882577425</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>0.699471598414795</c:v>
                 </c:pt>
               </c:numCache>
@@ -646,11 +664,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1068993680"/>
-        <c:axId val="1068995312"/>
+        <c:axId val="1116965392"/>
+        <c:axId val="1068310912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1068993680"/>
+        <c:axId val="1116965392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -706,12 +724,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1068995312"/>
+        <c:crossAx val="1068310912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1068995312"/>
+        <c:axId val="1068310912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +785,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1068993680"/>
+        <c:crossAx val="1116965392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1376,20 +1394,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1130300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3134,8 +3152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6575,10 +6593,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6684,16 +6702,16 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>49.129798253377203</v>
+        <v>18.374215920766101</v>
       </c>
       <c r="C4">
-        <v>18.966204643249501</v>
+        <v>7.3404917716979901</v>
       </c>
       <c r="D4">
-        <v>0.69976515485101998</v>
+        <v>0.68699544987523797</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -6711,36 +6729,36 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <v>0.72082782915015398</v>
+        <v>0.70717745486569705</v>
       </c>
       <c r="K4">
-        <v>0.67437252311756901</v>
+        <v>0.66292382210479905</v>
       </c>
       <c r="L4">
-        <v>0.70409511228533594</v>
+        <v>0.69088507265521704</v>
       </c>
       <c r="M4">
-        <v>1.6244200507758499</v>
+        <v>0.199029629380016</v>
       </c>
       <c r="N4">
-        <v>0.17835138844311499</v>
+        <v>0.15360987080013</v>
       </c>
       <c r="O4">
-        <v>1.9210852196653801E-2</v>
+        <v>1.8274624978587301E-2</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>55.345610380172701</v>
+        <v>20.9596690336863</v>
       </c>
       <c r="C5">
-        <v>21.001344998677499</v>
+        <v>8.5508293310801093</v>
       </c>
       <c r="D5">
-        <v>0.70343461030383003</v>
+        <v>0.69389402612652196</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -6758,36 +6776,36 @@
         <v>2</v>
       </c>
       <c r="J5">
-        <v>0.72148833113166</v>
+        <v>0.71158080140906999</v>
       </c>
       <c r="K5">
-        <v>0.68163804491413404</v>
+        <v>0.67459269044473802</v>
       </c>
       <c r="L5">
-        <v>0.70717745486569705</v>
+        <v>0.69550858652575898</v>
       </c>
       <c r="M5">
-        <v>0.67979027652456603</v>
+        <v>0.33728865664275998</v>
       </c>
       <c r="N5">
-        <v>0.83812879692982101</v>
+        <v>0.16189204455213499</v>
       </c>
       <c r="O5">
-        <v>1.64826776134906E-2</v>
+        <v>1.51434296454389E-2</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>62.507666031519499</v>
+        <v>49.129798253377203</v>
       </c>
       <c r="C6">
-        <v>25.524518728256201</v>
+        <v>18.966204643249501</v>
       </c>
       <c r="D6">
-        <v>0.70424189050344899</v>
+        <v>0.69976515485101998</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -6805,36 +6823,36 @@
         <v>2</v>
       </c>
       <c r="J6">
-        <v>0.72038749449581596</v>
+        <v>0.72082782915015398</v>
       </c>
       <c r="K6">
-        <v>0.68075737560546001</v>
+        <v>0.67437252311756901</v>
       </c>
       <c r="L6">
-        <v>0.71158080140906999</v>
+        <v>0.70409511228533594</v>
       </c>
       <c r="M6">
-        <v>1.01815835077146</v>
+        <v>1.6244200507758499</v>
       </c>
       <c r="N6">
-        <v>0.78181430810335995</v>
+        <v>0.17835138844311499</v>
       </c>
       <c r="O6">
-        <v>1.69908071375168E-2</v>
+        <v>1.9210852196653801E-2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B7">
-        <v>70.886246919631901</v>
+        <v>55.345610380172701</v>
       </c>
       <c r="C7">
-        <v>27.858318408330199</v>
+        <v>21.001344998677499</v>
       </c>
       <c r="D7">
-        <v>0.70262733010421197</v>
+        <v>0.70343461030383003</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -6852,36 +6870,36 @@
         <v>2</v>
       </c>
       <c r="J7">
-        <v>0.72082782915015398</v>
+        <v>0.72148833113166</v>
       </c>
       <c r="K7">
-        <v>0.67635402906208697</v>
+        <v>0.68163804491413404</v>
       </c>
       <c r="L7">
-        <v>0.71070013210039595</v>
+        <v>0.70717745486569705</v>
       </c>
       <c r="M7">
-        <v>1.6102048659556001</v>
+        <v>0.67979027652456603</v>
       </c>
       <c r="N7">
-        <v>0.43047200949786801</v>
+        <v>0.83812879692982101</v>
       </c>
       <c r="O7">
-        <v>1.9032556714229099E-2</v>
+        <v>1.64826776134906E-2</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B8">
-        <v>80.666984637578295</v>
+        <v>31.058151404062901</v>
       </c>
       <c r="C8">
-        <v>30.5815454324086</v>
+        <v>12.0565579732259</v>
       </c>
       <c r="D8">
-        <v>0.70270071921326804</v>
+        <v>0.70402172317627998</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -6899,36 +6917,36 @@
         <v>2</v>
       </c>
       <c r="J8">
-        <v>0.72126816380449099</v>
+        <v>0.72214883311316602</v>
       </c>
       <c r="K8">
-        <v>0.67789520035226702</v>
+        <v>0.68295904887714598</v>
       </c>
       <c r="L8">
-        <v>0.708938793483047</v>
+        <v>0.70695728753852904</v>
       </c>
       <c r="M8">
-        <v>2.6150282040022801</v>
+        <v>0.29050021277173099</v>
       </c>
       <c r="N8">
-        <v>0.64061370427439501</v>
+        <v>0.16937177658195099</v>
       </c>
       <c r="O8">
-        <v>1.8248080585885101E-2</v>
+        <v>1.6133256557188801E-2</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B9">
-        <v>48.892688274383502</v>
+        <v>62.507666031519499</v>
       </c>
       <c r="C9">
-        <v>18.638858636220199</v>
+        <v>25.524518728256201</v>
       </c>
       <c r="D9">
-        <v>0.702553940995156</v>
+        <v>0.70424189050344899</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -6937,45 +6955,45 @@
         <v>0.01</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I9">
         <v>2</v>
       </c>
       <c r="J9">
-        <v>0.71598414795244303</v>
+        <v>0.72038749449581596</v>
       </c>
       <c r="K9">
-        <v>0.68295904887714598</v>
+        <v>0.68075737560546001</v>
       </c>
       <c r="L9">
-        <v>0.708718626155878</v>
+        <v>0.71158080140906999</v>
       </c>
       <c r="M9">
-        <v>1.5782904165282099</v>
+        <v>1.01815835077146</v>
       </c>
       <c r="N9">
-        <v>0.323575529052327</v>
+        <v>0.78181430810335995</v>
       </c>
       <c r="O9">
-        <v>1.4169610664644601E-2</v>
+        <v>1.69908071375168E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B10">
-        <v>53.949284315109203</v>
+        <v>70.886246919631901</v>
       </c>
       <c r="C10">
-        <v>20.269028504689501</v>
+        <v>27.858318408330199</v>
       </c>
       <c r="D10">
-        <v>0.701599882577425</v>
+        <v>0.70262733010421197</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -6984,45 +7002,45 @@
         <v>0.01</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="J10">
-        <v>0.71334214002642005</v>
+        <v>0.72082782915015398</v>
       </c>
       <c r="K10">
-        <v>0.68229854689563996</v>
+        <v>0.67635402906208697</v>
       </c>
       <c r="L10">
-        <v>0.70915896081021501</v>
+        <v>0.71070013210039595</v>
       </c>
       <c r="M10">
-        <v>1.6475723808996601</v>
+        <v>1.6102048659556001</v>
       </c>
       <c r="N10">
-        <v>0.28279824725887998</v>
+        <v>0.43047200949786801</v>
       </c>
       <c r="O10">
-        <v>1.37545366192255E-2</v>
+        <v>1.9032556714229099E-2</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B11">
-        <v>60.1429108778635</v>
+        <v>80.666984637578295</v>
       </c>
       <c r="C11">
-        <v>22.070303599039701</v>
+        <v>30.5815454324086</v>
       </c>
       <c r="D11">
-        <v>0.699471598414795</v>
+        <v>0.70270071921326804</v>
       </c>
       <c r="E11">
         <v>5</v>
@@ -7031,110 +7049,275 @@
         <v>0.01</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="J11">
+        <v>0.72126816380449099</v>
+      </c>
+      <c r="K11">
+        <v>0.67789520035226702</v>
+      </c>
+      <c r="L11">
+        <v>0.708938793483047</v>
+      </c>
+      <c r="M11">
+        <v>2.6150282040022801</v>
+      </c>
+      <c r="N11">
+        <v>0.64061370427439501</v>
+      </c>
+      <c r="O11">
+        <v>1.8248080585885101E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>48.892688274383502</v>
+      </c>
+      <c r="C12">
+        <v>18.638858636220199</v>
+      </c>
+      <c r="D12">
+        <v>0.702553940995156</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>0.01</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>0.71598414795244303</v>
+      </c>
+      <c r="K12">
+        <v>0.68295904887714598</v>
+      </c>
+      <c r="L12">
+        <v>0.708718626155878</v>
+      </c>
+      <c r="M12">
+        <v>1.5782904165282099</v>
+      </c>
+      <c r="N12">
+        <v>0.323575529052327</v>
+      </c>
+      <c r="O12">
+        <v>1.4169610664644601E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>53.949284315109203</v>
+      </c>
+      <c r="C13">
+        <v>20.269028504689501</v>
+      </c>
+      <c r="D13">
+        <v>0.701599882577425</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>0.01</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>0.71334214002642005</v>
+      </c>
+      <c r="K13">
+        <v>0.68229854689563996</v>
+      </c>
+      <c r="L13">
+        <v>0.70915896081021501</v>
+      </c>
+      <c r="M13">
+        <v>1.6475723808996601</v>
+      </c>
+      <c r="N13">
+        <v>0.28279824725887998</v>
+      </c>
+      <c r="O13">
+        <v>1.37545366192255E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>60.1429108778635</v>
+      </c>
+      <c r="C14">
+        <v>22.070303599039701</v>
+      </c>
+      <c r="D14">
+        <v>0.699471598414795</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>0.01</v>
+      </c>
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
         <v>0.71246147071774502</v>
       </c>
-      <c r="K11">
+      <c r="K14">
         <v>0.67767503302509902</v>
       </c>
-      <c r="L11">
+      <c r="L14">
         <v>0.70827829150154098</v>
       </c>
-      <c r="M11">
+      <c r="M14">
         <v>2.3367847279117901</v>
       </c>
-      <c r="N11">
+      <c r="N14">
         <v>0.37997430599276599</v>
       </c>
-      <c r="O11">
+      <c r="O14">
         <v>1.5506825253829201E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>9</v>
-      </c>
-      <c r="B15">
-        <v>0.68376632907676504</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>0.69976515485101998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>0.70343461030383003</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B18">
-        <v>0.70424189050344899</v>
+        <v>0.68376632907676504</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B19">
-        <v>0.70262733010421197</v>
+        <v>0.68699544987523797</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B20">
-        <v>0.70270071921326804</v>
+        <v>0.69389402612652196</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B21">
-        <v>0.702553940995156</v>
+        <v>0.69976515485101998</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>0.701599882577425</v>
+        <v>0.70343461030383003</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>0.70402172317627998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>0.70424189050344899</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0.70262733010421197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0.70270071921326804</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>0.702553940995156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>0.701599882577425</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>31</v>
       </c>
-      <c r="B23">
+      <c r="B29">
         <v>0.699471598414795</v>
       </c>
     </row>
@@ -7149,7 +7332,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O7"/>
+      <selection activeCell="B5" sqref="B5:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7502,7 +7685,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O7"/>
+      <selection activeCell="B5" sqref="B5:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8566,7 +8749,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O7"/>
+      <selection activeCell="B5" sqref="B5:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
minor code adjustments for metrics
</commit_message>
<xml_diff>
--- a/Project/Datasets/GridScores/Combined.xlsx
+++ b/Project/Datasets/GridScores/Combined.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="440" windowWidth="24680" windowHeight="15560" tabRatio="500" firstSheet="1" activeTab="13"/>
+    <workbookView xWindow="920" yWindow="440" windowWidth="24680" windowHeight="15560" tabRatio="500" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="9" sheetId="3" r:id="rId1"/>
@@ -3152,53 +3152,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -6595,8 +6595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
set predictor to use size50 model available on git
</commit_message>
<xml_diff>
--- a/Project/Datasets/GridScores/Combined.xlsx
+++ b/Project/Datasets/GridScores/Combined.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="440" windowWidth="24680" windowHeight="15560" tabRatio="500" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="920" yWindow="440" windowWidth="24680" windowHeight="15560" tabRatio="500" firstSheet="3" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="9" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <sheet name="29" sheetId="11" r:id="rId11"/>
     <sheet name="31" sheetId="12" r:id="rId12"/>
     <sheet name="Big Compariso" sheetId="13" r:id="rId13"/>
-    <sheet name="WindowComparison" sheetId="9" r:id="rId14"/>
+    <sheet name="Sheet7" sheetId="19" r:id="rId14"/>
+    <sheet name="Sheet8" sheetId="20" r:id="rId15"/>
+    <sheet name="WindowComparison" sheetId="9" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_11_improved" localSheetId="1">'11'!$A$1:$O$7</definedName>
@@ -311,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="49">
   <si>
     <t>mean_fit_time</t>
   </si>
@@ -390,6 +392,75 @@
   <si>
     <t>Window Size</t>
   </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Mean fit time</t>
+  </si>
+  <si>
+    <t>Mean test score</t>
+  </si>
+  <si>
+    <t>WinSize 9</t>
+  </si>
+  <si>
+    <t>WinSize 11</t>
+  </si>
+  <si>
+    <t>WinSize 13</t>
+  </si>
+  <si>
+    <t>WinSize 15</t>
+  </si>
+  <si>
+    <t>WinSize 17</t>
+  </si>
+  <si>
+    <t>WinSize 19</t>
+  </si>
+  <si>
+    <t>WinSize 21</t>
+  </si>
+  <si>
+    <t>WinSize 23</t>
+  </si>
+  <si>
+    <t>WinSize 25</t>
+  </si>
+  <si>
+    <t>WinSize 27</t>
+  </si>
+  <si>
+    <t>WinSize 29</t>
+  </si>
+  <si>
+    <t>WinSize 31</t>
+  </si>
+  <si>
+    <t>C=1, Gamma = 0.001</t>
+  </si>
+  <si>
+    <t>C=1, Gamma = 0.01</t>
+  </si>
+  <si>
+    <t>C=5, Gamma = 0.001</t>
+  </si>
+  <si>
+    <t>C=5, Gamma = 0.01</t>
+  </si>
+  <si>
+    <t>C=10, Gamma = 0.001</t>
+  </si>
+  <si>
+    <t>C=10, Gamma = 0.01</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
 </sst>
 </file>
 
@@ -435,15 +506,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -451,20 +528,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -484,14 +586,39 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="104"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="4"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GridSearch</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -525,6 +652,1626 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C=1, Gamma = 0.001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:tint val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$G$1:$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>WinSize 9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WinSize 11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WinSize 13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>WinSize 15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>WinSize 17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>WinSize 19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WinSize 21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>WinSize 23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>WinSize 25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>WinSize 27</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>WinSize 29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>WinSize 31</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$G$2:$R$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.575517393218846</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.579113459562601</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.583223249669749</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58571847937766</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.587479818</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.589754880375752</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.590635549684426</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.591296051665932</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.593130779392338</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.594231616028181</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.59540584177308</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.595552619991193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C=1, Gamma = 0.01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:tint val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$G$1:$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>WinSize 9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WinSize 11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WinSize 13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>WinSize 15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>WinSize 17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>WinSize 19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WinSize 21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>WinSize 23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>WinSize 25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>WinSize 27</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>WinSize 29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>WinSize 31</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$G$3:$R$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.684573609276383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.686481726111845</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.687655951856744</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.690958461764274</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.693894026</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.697343314252165</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.697563481579333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.696829590488771</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.696536034052546</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.697636870688389</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.697783648906502</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.698150594451783</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C=5, Gamma = 0.001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:tint val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$G$1:$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>WinSize 9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WinSize 11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WinSize 13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>WinSize 15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>WinSize 17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>WinSize 19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WinSize 21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>WinSize 23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>WinSize 25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>WinSize 27</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>WinSize 29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>WinSize 31</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$G$4:$R$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.683619550858652</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.684500220167327</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6877293409658</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69161896374578</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.693160135</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.694114193453691</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.695508586525759</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.695435197416703</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.695655364743872</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.693820637017466</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.696536034052546</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.695508586525759</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C=5, Gamma = 0.01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:shade val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$G$1:$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>WinSize 9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WinSize 11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WinSize 13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>WinSize 15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>WinSize 17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>WinSize 19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WinSize 21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>WinSize 23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>WinSize 25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>WinSize 27</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>WinSize 29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>WinSize 31</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$G$5:$R$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.683766329076765</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.686995449875238</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.693894026126522</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69976515485102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70343461</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.70402172317628</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.704241890503449</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.702627330104212</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.702700719213268</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.702553940995156</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.701599882577425</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.699471598414795</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$F$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C=10, Gamma = 0.001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:shade val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$G$1:$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>WinSize 9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WinSize 11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WinSize 13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>WinSize 15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>WinSize 17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>WinSize 19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WinSize 21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>WinSize 23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>WinSize 25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>WinSize 27</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>WinSize 29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>WinSize 31</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$G$6:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.683619550858652</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.684940554821664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.686922060766182</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.688463232056362</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.691545575</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.694627917217085</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.695802142961984</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.696022310289153</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.697123146924996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.696169088507265</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.696609423161602</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.695288419198591</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C=10, Gamma = 0.01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$G$1:$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>WinSize 9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WinSize 11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WinSize 13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>WinSize 15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>WinSize 17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>WinSize 19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WinSize 21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>WinSize 23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>WinSize 25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>WinSize 27</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>WinSize 29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>WinSize 31</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$G$7:$R$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.68831645383825</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.697710259797446</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.701086158814032</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.704315279612505</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.705195949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.709158960810215</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.706223396447967</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.703874944958168</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.703067664758549</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.703214442976662</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.702920886540437</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.699985322178188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1149215488"/>
+        <c:axId val="1149217264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1149215488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1149217264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1149217264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.55"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="wordArtVert" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mean Test Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="wordArtVert" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1149215488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GridSearch</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet8!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WinSize 17</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet8!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>C=1, Gamma = 0.001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>C=1, Gamma = 0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C=5, Gamma = 0.001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>C=5, Gamma = 0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>C=10, Gamma = 0.001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>C=10, Gamma = 0.01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet8!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.587479818</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.693894026</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.693160135</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70343461</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.691545575</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.705195949</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet8!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WinSize 19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet8!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>C=1, Gamma = 0.001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>C=1, Gamma = 0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C=5, Gamma = 0.001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>C=5, Gamma = 0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>C=10, Gamma = 0.001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>C=10, Gamma = 0.01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet8!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.589754880375752</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.697343314252165</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.694114193453691</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70402172317628</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.694627917217085</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.709158960810215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet8!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WinSize 21</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet8!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>C=1, Gamma = 0.001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>C=1, Gamma = 0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C=5, Gamma = 0.001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>C=5, Gamma = 0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>C=10, Gamma = 0.001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>C=10, Gamma = 0.01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet8!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.590635549684426</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.697563481579333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.695508586525759</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.704241890503449</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.695802142961984</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.706223396447967</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet8!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WinSize 23</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="98500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet8!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>C=1, Gamma = 0.001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>C=1, Gamma = 0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C=5, Gamma = 0.001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>C=5, Gamma = 0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>C=10, Gamma = 0.001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>C=10, Gamma = 0.01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet8!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.591296051665932</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.696829590488771</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.695435197416703</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.702627330104212</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.696022310289153</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.703874944958168</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1118140928"/>
+        <c:axId val="1118532752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1118140928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1118532752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1118532752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.55"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="wordArtVert" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mean Test Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="wordArtVert" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1118140928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.05"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -550,15 +2297,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1">
+                  <a:alpha val="90000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -674,20 +2423,63 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Window Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -749,6 +2541,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="wordArtVert" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mean Test Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="wordArtVert" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -835,6 +2683,39 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="22">
+  <a:schemeClr val="accent2"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -875,6 +2756,1012 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1394,16 +4281,86 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1130300</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3152,8 +6109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="A2:O74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6593,10 +9550,1478 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:R7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="18" width="7.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>0.57551739321884599</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1E-3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2">
+        <v>0.57551739321884599</v>
+      </c>
+      <c r="H2">
+        <v>0.57911345956260096</v>
+      </c>
+      <c r="I2">
+        <v>0.58322324966974903</v>
+      </c>
+      <c r="J2">
+        <v>0.58571847937765997</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.58747981800000004</v>
+      </c>
+      <c r="L2">
+        <v>0.58975488037575197</v>
+      </c>
+      <c r="M2">
+        <v>0.590635549684426</v>
+      </c>
+      <c r="N2">
+        <v>0.59129605166593202</v>
+      </c>
+      <c r="O2">
+        <v>0.59313077939233805</v>
+      </c>
+      <c r="P2">
+        <v>0.59423161602818098</v>
+      </c>
+      <c r="Q2">
+        <v>0.59540584177307998</v>
+      </c>
+      <c r="R2">
+        <v>0.59555261999119302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3">
+        <v>0.684573609276383</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.01</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3">
+        <v>0.684573609276383</v>
+      </c>
+      <c r="H3">
+        <v>0.68648172611184499</v>
+      </c>
+      <c r="I3">
+        <v>0.687655951856744</v>
+      </c>
+      <c r="J3">
+        <v>0.690958461764274</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.69389402600000005</v>
+      </c>
+      <c r="L3">
+        <v>0.697343314252165</v>
+      </c>
+      <c r="M3">
+        <v>0.69756348157933301</v>
+      </c>
+      <c r="N3">
+        <v>0.69682959048877102</v>
+      </c>
+      <c r="O3">
+        <v>0.69653603405254605</v>
+      </c>
+      <c r="P3">
+        <v>0.69763687068838898</v>
+      </c>
+      <c r="Q3">
+        <v>0.69778364890650202</v>
+      </c>
+      <c r="R3">
+        <v>0.69815059445178296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4">
+        <v>0.683619550858652</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1E-3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4">
+        <v>0.683619550858652</v>
+      </c>
+      <c r="H4">
+        <v>0.68450022016732703</v>
+      </c>
+      <c r="I4">
+        <v>0.68772934096579996</v>
+      </c>
+      <c r="J4">
+        <v>0.69161896374578002</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.69316013499999996</v>
+      </c>
+      <c r="L4">
+        <v>0.69411419345369096</v>
+      </c>
+      <c r="M4">
+        <v>0.69550858652575898</v>
+      </c>
+      <c r="N4">
+        <v>0.69543519741670301</v>
+      </c>
+      <c r="O4">
+        <v>0.69565536474387202</v>
+      </c>
+      <c r="P4">
+        <v>0.69382063701746599</v>
+      </c>
+      <c r="Q4">
+        <v>0.69653603405254605</v>
+      </c>
+      <c r="R4">
+        <v>0.69550858652575898</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5">
+        <v>0.68376632907676504</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>0.01</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5">
+        <v>0.68376632907676504</v>
+      </c>
+      <c r="H5">
+        <v>0.68699544987523797</v>
+      </c>
+      <c r="I5">
+        <v>0.69389402612652196</v>
+      </c>
+      <c r="J5">
+        <v>0.69976515485101998</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.70343460999999996</v>
+      </c>
+      <c r="L5">
+        <v>0.70402172317627998</v>
+      </c>
+      <c r="M5">
+        <v>0.70424189050344899</v>
+      </c>
+      <c r="N5">
+        <v>0.70262733010421197</v>
+      </c>
+      <c r="O5">
+        <v>0.70270071921326804</v>
+      </c>
+      <c r="P5">
+        <v>0.702553940995156</v>
+      </c>
+      <c r="Q5">
+        <v>0.701599882577425</v>
+      </c>
+      <c r="R5">
+        <v>0.699471598414795</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6">
+        <v>0.683619550858652</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>1E-3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6">
+        <v>0.683619550858652</v>
+      </c>
+      <c r="H6">
+        <v>0.68494055482166405</v>
+      </c>
+      <c r="I6">
+        <v>0.68692206076618201</v>
+      </c>
+      <c r="J6">
+        <v>0.68846323205636195</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.69154557500000002</v>
+      </c>
+      <c r="L6">
+        <v>0.69462791721708494</v>
+      </c>
+      <c r="M6">
+        <v>0.69580214296198395</v>
+      </c>
+      <c r="N6">
+        <v>0.69602231028915296</v>
+      </c>
+      <c r="O6">
+        <v>0.697123146924996</v>
+      </c>
+      <c r="P6">
+        <v>0.696169088507265</v>
+      </c>
+      <c r="Q6">
+        <v>0.69660942316160201</v>
+      </c>
+      <c r="R6">
+        <v>0.69528841919859097</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
+      <c r="B7">
+        <v>0.68831645383825002</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>0.01</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7">
+        <v>0.68831645383825002</v>
+      </c>
+      <c r="H7">
+        <v>0.69771025979744605</v>
+      </c>
+      <c r="I7">
+        <v>0.70108615881403202</v>
+      </c>
+      <c r="J7">
+        <v>0.70431527961250495</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.70519594900000004</v>
+      </c>
+      <c r="L7">
+        <v>0.70915896081021501</v>
+      </c>
+      <c r="M7">
+        <v>0.70622339644796694</v>
+      </c>
+      <c r="N7">
+        <v>0.70387494495816805</v>
+      </c>
+      <c r="O7">
+        <v>0.70306766475854898</v>
+      </c>
+      <c r="P7">
+        <v>0.70321444297666202</v>
+      </c>
+      <c r="Q7">
+        <v>0.70292088654043705</v>
+      </c>
+      <c r="R7">
+        <v>0.69998532217818799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.57911345956260096</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9">
+        <v>0.68648172611184499</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10">
+        <v>0.68450022016732703</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>1E-3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1">
+        <v>11</v>
+      </c>
+      <c r="I10" s="1">
+        <v>13</v>
+      </c>
+      <c r="J10" s="1">
+        <v>15</v>
+      </c>
+      <c r="K10" s="1">
+        <v>17</v>
+      </c>
+      <c r="L10" s="1">
+        <v>19</v>
+      </c>
+      <c r="M10" s="1">
+        <v>21</v>
+      </c>
+      <c r="N10" s="1">
+        <v>23</v>
+      </c>
+      <c r="O10" s="1">
+        <v>25</v>
+      </c>
+      <c r="P10" s="1">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>29</v>
+      </c>
+      <c r="R10" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11">
+        <v>0.68699544987523797</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12">
+        <v>0.68494055482166405</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13">
+        <v>0.69771025979744605</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0.58322324966974903</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.687655951856744</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>0.68772934096579996</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>0.69389402612652196</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>0.68692206076618201</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>0.70108615881403202</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>0.58571847937765997</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>0.690958461764274</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>0.69161896374578002</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>0.69976515485101998</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>15</v>
+      </c>
+      <c r="B24">
+        <v>0.68846323205636195</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>0.70431527961250495</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>17</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.58747981800000004</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>17</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.69389402600000005</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>17</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.69316013499999996</v>
+      </c>
+      <c r="C28" s="2">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.70343460999999996</v>
+      </c>
+      <c r="C29" s="2">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>17</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.69154557500000002</v>
+      </c>
+      <c r="C30" s="2">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>17</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.70519594900000004</v>
+      </c>
+      <c r="C31" s="2">
+        <v>10</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>19</v>
+      </c>
+      <c r="B32">
+        <v>0.58975488037575197</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>0.697343314252165</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>19</v>
+      </c>
+      <c r="B34">
+        <v>0.69411419345369096</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>19</v>
+      </c>
+      <c r="B35">
+        <v>0.70402172317627998</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <v>0.69462791721708494</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>19</v>
+      </c>
+      <c r="B37">
+        <v>0.70915896081021501</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <v>0.590635549684426</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>21</v>
+      </c>
+      <c r="B39">
+        <v>0.69756348157933301</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>21</v>
+      </c>
+      <c r="B40">
+        <v>0.69550858652575898</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>21</v>
+      </c>
+      <c r="B41">
+        <v>0.70424189050344899</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>21</v>
+      </c>
+      <c r="B42">
+        <v>0.69580214296198395</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>21</v>
+      </c>
+      <c r="B43">
+        <v>0.70622339644796694</v>
+      </c>
+      <c r="C43">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>23</v>
+      </c>
+      <c r="B44">
+        <v>0.59129605166593202</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>0.69682959048877102</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>23</v>
+      </c>
+      <c r="B46">
+        <v>0.69543519741670301</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>23</v>
+      </c>
+      <c r="B47">
+        <v>0.70262733010421197</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>23</v>
+      </c>
+      <c r="B48">
+        <v>0.69602231028915296</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>23</v>
+      </c>
+      <c r="B49">
+        <v>0.70387494495816805</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>25</v>
+      </c>
+      <c r="B50">
+        <v>0.59313077939233805</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>25</v>
+      </c>
+      <c r="B51">
+        <v>0.69653603405254605</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>25</v>
+      </c>
+      <c r="B52">
+        <v>0.69565536474387202</v>
+      </c>
+      <c r="C52">
+        <v>5</v>
+      </c>
+      <c r="D52">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>25</v>
+      </c>
+      <c r="B53">
+        <v>0.70270071921326804</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>25</v>
+      </c>
+      <c r="B54">
+        <v>0.697123146924996</v>
+      </c>
+      <c r="C54">
+        <v>10</v>
+      </c>
+      <c r="D54">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>25</v>
+      </c>
+      <c r="B55">
+        <v>0.70306766475854898</v>
+      </c>
+      <c r="C55">
+        <v>10</v>
+      </c>
+      <c r="D55">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>27</v>
+      </c>
+      <c r="B56">
+        <v>0.59423161602818098</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>27</v>
+      </c>
+      <c r="B57">
+        <v>0.69763687068838898</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>27</v>
+      </c>
+      <c r="B58">
+        <v>0.69382063701746599</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+      <c r="D58">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>27</v>
+      </c>
+      <c r="B59">
+        <v>0.702553940995156</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+      <c r="D59">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>27</v>
+      </c>
+      <c r="B60">
+        <v>0.696169088507265</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
+      </c>
+      <c r="D60">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>27</v>
+      </c>
+      <c r="B61">
+        <v>0.70321444297666202</v>
+      </c>
+      <c r="C61">
+        <v>10</v>
+      </c>
+      <c r="D61">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>29</v>
+      </c>
+      <c r="B62">
+        <v>0.59540584177307998</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>29</v>
+      </c>
+      <c r="B63">
+        <v>0.69778364890650202</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>29</v>
+      </c>
+      <c r="B64">
+        <v>0.69653603405254605</v>
+      </c>
+      <c r="C64">
+        <v>5</v>
+      </c>
+      <c r="D64">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>29</v>
+      </c>
+      <c r="B65">
+        <v>0.701599882577425</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>29</v>
+      </c>
+      <c r="B66">
+        <v>0.69660942316160201</v>
+      </c>
+      <c r="C66">
+        <v>10</v>
+      </c>
+      <c r="D66">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>29</v>
+      </c>
+      <c r="B67">
+        <v>0.70292088654043705</v>
+      </c>
+      <c r="C67">
+        <v>10</v>
+      </c>
+      <c r="D67">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>31</v>
+      </c>
+      <c r="B68">
+        <v>0.59555261999119302</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>31</v>
+      </c>
+      <c r="B69">
+        <v>0.69815059445178296</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>31</v>
+      </c>
+      <c r="B70">
+        <v>0.69550858652575898</v>
+      </c>
+      <c r="C70">
+        <v>5</v>
+      </c>
+      <c r="D70">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>31</v>
+      </c>
+      <c r="B71">
+        <v>0.699471598414795</v>
+      </c>
+      <c r="C71">
+        <v>5</v>
+      </c>
+      <c r="D71">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>31</v>
+      </c>
+      <c r="B72">
+        <v>0.69528841919859097</v>
+      </c>
+      <c r="C72">
+        <v>10</v>
+      </c>
+      <c r="D72">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>31</v>
+      </c>
+      <c r="B73">
+        <v>0.69998532217818799</v>
+      </c>
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="D73">
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.58747981800000004</v>
+      </c>
+      <c r="C2">
+        <v>0.58975488037575197</v>
+      </c>
+      <c r="D2">
+        <v>0.590635549684426</v>
+      </c>
+      <c r="E2">
+        <v>0.59129605166593202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.69389402600000005</v>
+      </c>
+      <c r="C3">
+        <v>0.697343314252165</v>
+      </c>
+      <c r="D3">
+        <v>0.69756348157933301</v>
+      </c>
+      <c r="E3">
+        <v>0.69682959048877102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.69316013499999996</v>
+      </c>
+      <c r="C4">
+        <v>0.69411419345369096</v>
+      </c>
+      <c r="D4">
+        <v>0.69550858652575898</v>
+      </c>
+      <c r="E4">
+        <v>0.69543519741670301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.70343460999999996</v>
+      </c>
+      <c r="C5">
+        <v>0.70402172317627998</v>
+      </c>
+      <c r="D5">
+        <v>0.70424189050344899</v>
+      </c>
+      <c r="E5">
+        <v>0.70262733010421197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.69154557500000002</v>
+      </c>
+      <c r="C6">
+        <v>0.69462791721708494</v>
+      </c>
+      <c r="D6">
+        <v>0.69580214296198395</v>
+      </c>
+      <c r="E6">
+        <v>0.69602231028915296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.70519594900000004</v>
+      </c>
+      <c r="C7">
+        <v>0.70915896081021501</v>
+      </c>
+      <c r="D7">
+        <v>0.70622339644796694</v>
+      </c>
+      <c r="E7">
+        <v>0.70387494495816805</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9099,19 +13524,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -9443,6 +13868,104 @@
       </c>
       <c r="O7">
         <v>1.7756221563786499E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.590635549684426</v>
+      </c>
+      <c r="E10" s="4">
+        <v>72.981989622116004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.69756348157933301</v>
+      </c>
+      <c r="E11" s="4">
+        <v>64.415209611256898</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B12" s="3">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.69550858652575898</v>
+      </c>
+      <c r="E12" s="4">
+        <v>65.085086345672593</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.70424189050344899</v>
+      </c>
+      <c r="E13" s="4">
+        <v>62.507666031519499</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B14" s="3">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.69580214296198395</v>
+      </c>
+      <c r="E14" s="4">
+        <v>61.620828866958597</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B15" s="3">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.70622339644796694</v>
+      </c>
+      <c r="E15" s="4">
+        <v>82.250488440195696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Diary update and minor code ammendments
</commit_message>
<xml_diff>
--- a/Project/Datasets/GridScores/Combined.xlsx
+++ b/Project/Datasets/GridScores/Combined.xlsx
@@ -1612,10 +1612,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1698,9 +1698,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:tint val="88500"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1778,9 +1776,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:tint val="55000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1858,9 +1854,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:tint val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1938,9 +1932,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:tint val="98500"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent4"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2070,7 +2062,7 @@
         <c:axId val="1118532752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.55"/>
+          <c:min val="0.58"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2090,7 +2082,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="wordArtVert" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2123,7 +2115,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="wordArtVert" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -2420,6 +2412,8 @@
         <c:axId val="1116965392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="31.0"/>
+          <c:min val="9.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2544,7 +2538,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="wordArtVert" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2577,7 +2571,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="wordArtVert" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -2689,28 +2683,41 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
-  <a:schemeClr val="dk1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
   <cs:variation>
-    <a:tint val="88500"/>
+    <a:lumMod val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="55000"/>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="75000"/>
+    <a:lumMod val="80000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="98500"/>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="30000"/>
+    <a:lumMod val="50000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="60000"/>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="80000"/>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
@@ -10886,7 +10893,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11020,8 +11027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>